<commit_message>
Now normalizes FA, INV, and LAND, and then calculates economic depreciation rates.  Note that INV and LAND have roughly a depreciation rate of zero.  Missing depreciation rates for FA are currently given a default of zero.
</commit_message>
<xml_diff>
--- a/Data/Calibration/DepreciationParameters/Program/data/Inventories/Crosswalk/Inventories_Crosswalk.xlsx
+++ b/Data/Calibration/DepreciationParameters/Program/data/Inventories/Crosswalk/Inventories_Crosswalk.xlsx
@@ -77,9 +77,6 @@
     <t>31.32.33</t>
   </si>
   <si>
-    <t>45.49.51.52.53.54.55.56.61.62.71.72.81.92</t>
-  </si>
-  <si>
     <t>311.312.313.314.315.316.322.323.324.325.326</t>
   </si>
   <si>
@@ -132,6 +129,9 @@
   </si>
   <si>
     <t>List</t>
+  </si>
+  <si>
+    <t>49.51.52.53.54.55.56.61.62.71.72.81.92</t>
   </si>
 </sst>
 </file>
@@ -458,14 +458,14 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s">
         <v>13</v>
@@ -476,7 +476,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -487,7 +487,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -498,7 +498,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
@@ -509,7 +509,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
@@ -520,29 +520,29 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
         <v>3</v>
@@ -553,7 +553,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
@@ -564,7 +564,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
         <v>8</v>
@@ -575,7 +575,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11" t="s">
         <v>4</v>
@@ -586,7 +586,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B12" t="s">
         <v>9</v>
@@ -597,7 +597,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
@@ -608,7 +608,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B14" t="s">
         <v>11</v>
@@ -619,7 +619,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B15" t="s">
         <v>12</v>
@@ -630,13 +630,13 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B16" t="s">
         <v>5</v>
       </c>
       <c r="C16" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>